<commit_message>
Changed "assay" to "bc_set" for clarity
</commit_message>
<xml_diff>
--- a/data/plate-maps/200402_run04/SARS-CoV-2_run04.xlsx
+++ b/data/plate-maps/200402_run04/SARS-CoV-2_run04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassc\Dropbox (Octant)\Scott\platform_SARS-CoV-2\Run04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B59CEA-3B95-4CE3-8325-6FD9C2B0DC85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EED424-D5F7-4F00-B7B5-3F1F1E4F4C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_notes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="143">
   <si>
     <t>plate maps for initial nCoV seq-based screening expt</t>
   </si>
@@ -176,15 +176,6 @@
   </si>
   <si>
     <t>HEK293</t>
-  </si>
-  <si>
-    <t>assay</t>
-  </si>
-  <si>
-    <t>N1_RPP30</t>
-  </si>
-  <si>
-    <t>S2_RPP30</t>
   </si>
   <si>
     <t>GAGTCTTC</t>
@@ -473,6 +464,12 @@
   </si>
   <si>
     <t>TTTGGAAC</t>
+  </si>
+  <si>
+    <t>bc_set</t>
+  </si>
+  <si>
+    <t>N1_S2_RPP30</t>
   </si>
 </sst>
 </file>
@@ -2199,8 +2196,8 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2229,7 +2226,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>6</v>
@@ -2255,7 +2252,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="G2" s="1">
         <v>64</v>
@@ -2281,7 +2278,7 @@
         <v>100</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="G3" s="1">
         <v>55</v>
@@ -3389,76 +3386,76 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3466,76 +3463,76 @@
         <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3543,76 +3540,76 @@
         <v>20</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="W4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="X4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="Y4" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y4" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3620,76 +3617,76 @@
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="V5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="W5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3697,76 +3694,76 @@
         <v>23</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="X6" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="T6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="V6" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="X6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y6" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3774,76 +3771,76 @@
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="O7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="Q7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="R7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="T7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="U7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="V7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="W7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="X7" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="Y7" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="V7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="X7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y7" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3851,76 +3848,76 @@
         <v>25</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="N8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="O8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="Q8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="R8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="T8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="U8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="V8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="W8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="X8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="Y8" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="T8" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="V8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="W8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="X8" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y8" s="9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3928,76 +3925,76 @@
         <v>26</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="O9" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="Q9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="R9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="T9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="U9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="V9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="W9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="X9" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="Y9" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="T9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="V9" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="X9" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y9" s="9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4005,76 +4002,76 @@
         <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="R10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="T10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="U10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="V10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="W10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="X10" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="Y10" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="V10" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="X10" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y10" s="9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4082,76 +4079,76 @@
         <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="L11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="M11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="N11" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="Q11" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="R11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="T11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="U11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="V11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="W11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="X11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="Y11" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="T11" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="V11" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W11" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="X11" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y11" s="9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4159,76 +4156,76 @@
         <v>29</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="K12" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="O12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="R12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="T12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="U12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="V12" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="W12" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="X12" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="Y12" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="U12" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="V12" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="X12" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y12" s="9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4236,76 +4233,76 @@
         <v>31</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="K13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="L13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="M13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="Q13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="R13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="T13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="U13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="V13" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="W13" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="X13" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="Y13" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="T13" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="U13" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="V13" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="W13" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="X13" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y13" s="9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4313,76 +4310,76 @@
         <v>32</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="K14" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="L14" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="M14" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="N14" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="O14" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="P14" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="Q14" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="R14" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="S14" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="T14" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="U14" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="V14" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="Q14" s="9" t="s">
+      <c r="W14" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="X14" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="Y14" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="T14" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="U14" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="V14" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="W14" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="X14" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y14" s="9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4390,76 +4387,76 @@
         <v>34</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="J15" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="L15" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="M15" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="N15" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="O15" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="P15" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="Q15" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="R15" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="S15" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="T15" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="U15" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="V15" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="W15" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="R15" s="9" t="s">
+      <c r="X15" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="S15" s="9" t="s">
+      <c r="Y15" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="T15" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="U15" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="V15" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="W15" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="X15" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y15" s="9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4467,76 +4464,76 @@
         <v>36</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="M16" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="N16" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="Q16" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="R16" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="S16" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="T16" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="U16" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="V16" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="Q16" s="9" t="s">
+      <c r="W16" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="R16" s="9" t="s">
+      <c r="X16" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="Y16" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="T16" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="U16" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="V16" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="W16" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="X16" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y16" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4544,76 +4541,76 @@
         <v>38</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="J17" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="K17" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="L17" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="M17" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="O17" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="Q17" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="R17" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="S17" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="T17" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="U17" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="V17" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="Q17" s="9" t="s">
+      <c r="W17" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="X17" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="S17" s="9" t="s">
+      <c r="Y17" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="T17" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="U17" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="V17" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="W17" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="X17" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y17" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9127,7 +9124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>

</xml_diff>